<commit_message>
Timesheet and Weekly Report
Added in time for stomach virus over last weekend under "illness"
wk-18.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Finance/Timesheets/James Oatley/Timesheet wk-18.xlsx
+++ b/Documents/Finance/Timesheets/James Oatley/Timesheet wk-18.xlsx
@@ -586,6 +586,41 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -601,42 +636,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -960,50 +960,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="36"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1012,26 +1012,26 @@
       <c r="A6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -1040,17 +1040,17 @@
       <c r="A8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="38">
+      <c r="F8" s="30"/>
+      <c r="G8" s="37">
         <v>41764</v>
       </c>
-      <c r="H8" s="39"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="10" t="s">
         <v>4</v>
       </c>
@@ -1192,14 +1192,16 @@
         <v>0</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4">
+        <v>6</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1211,14 +1213,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4">
+        <v>4</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1235,7 +1239,7 @@
       </c>
       <c r="D18" s="21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E18" s="21">
         <f t="shared" si="2"/>
@@ -1255,7 +1259,7 @@
       </c>
       <c r="I18" s="15">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -1326,22 +1330,22 @@
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="13">
         <f>I18</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="13">
         <f>I20</f>
         <v>62.5</v>
@@ -1349,74 +1353,59 @@
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:9" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="27" t="s">
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="28"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:9" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="34">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="45">
         <v>41771</v>
       </c>
-      <c r="E27" s="32"/>
+      <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="27" t="s">
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="28"/>
+      <c r="E28" s="41"/>
     </row>
     <row r="29" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
       <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A30:C30"/>
@@ -1427,6 +1416,21 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>